<commit_message>
se actualizan cards de seccion mis trabajos con imgs y urls definitivas
</commit_message>
<xml_diff>
--- a/assets/txts/gantt_proyecto.xlsx
+++ b/assets/txts/gantt_proyecto.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rodrigoquiroz/Desktop/portafolio/assets/txts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F355A9-7C43-FC44-B5CE-02B566EA4AB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DACE61-D995-B64F-8D8A-3233BECF26B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11580" yWindow="5460" windowWidth="28040" windowHeight="17440" xr2:uid="{C1D79A8D-4D62-E94C-84CF-61FD7516A90E}"/>
   </bookViews>
@@ -472,7 +472,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>